<commit_message>
Updated AND color-coded for fun
</commit_message>
<xml_diff>
--- a/HalbachPositions (version 1).xlsx
+++ b/HalbachPositions (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steph\Documents\GitHub\Hallbach_cylinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774A60B6-8163-48D9-AF12-EA37F54198B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD22E52-9BA8-44C2-B5FB-304753A8AC88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5A3979A9-2DE4-234A-B973-A6AC692A53E8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t># of magnets</t>
   </si>
@@ -79,12 +79,24 @@
   <si>
     <t>rotation per magnet (2B)</t>
   </si>
+  <si>
+    <t>cube edge</t>
+  </si>
+  <si>
+    <t>Cut depth</t>
+  </si>
+  <si>
+    <t>Ring height</t>
+  </si>
+  <si>
+    <t>≈5.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,13 +104,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -127,6 +205,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,7 +337,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.3970030474244572E-2"/>
+          <c:y val="6.513444610423022E-2"/>
+          <c:w val="0.93947598285519696"/>
+          <c:h val="0.92522003684530818"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -266,96 +385,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$O$14</c:f>
+              <c:f>Sheet1!$C$14:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4.75</c:v>
+                  <c:v>5.5175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.210517352263626</c:v>
+                  <c:v>22.53704516538064</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.3479208417492</c:v>
+                  <c:v>28.000307278913798</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.763960944970711</c:v>
+                  <c:v>24.482500000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.17548044745967</c:v>
+                  <c:v>18.44371694815252</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7500000000000009</c:v>
+                  <c:v>12.980454834619358</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-7.2398190008976631</c:v>
+                  <c:v>5.5175000000000018</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-22.449622391532699</c:v>
+                  <c:v>-7.4629548346193504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-28.033582288311202</c:v>
+                  <c:v>-23.961216948152504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-16.274855905701639</c:v>
+                  <c:v>-35.517499999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.7499999999999876</c:v>
+                  <c:v>-33.517807278913793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.210517352263608</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20.347920841749211</c:v>
+                  <c:v>-17.019545165380656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$O$15</c:f>
+              <c:f>Sheet1!$C$15:$N$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>27.25</c:v>
+                  <c:v>35.517499999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.153194644315338</c:v>
+                  <c:v>23.961216948152522</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31807170176606991</c:v>
+                  <c:v>7.4629548346193646</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.0037331483280685</c:v>
+                  <c:v>-5.5174999999999983</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-12.217533197753335</c:v>
+                  <c:v>-12.980454834619355</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-17.75</c:v>
+                  <c:v>-18.44371694815252</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-21.2525701025573</c:v>
+                  <c:v>-24.482499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-13.587693045106569</c:v>
+                  <c:v>-28.000307278913802</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9020315985445517</c:v>
+                  <c:v>-22.537045165380654</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.188231549119287</c:v>
+                  <c:v>-5.5175000000000116</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.250000000000007</c:v>
+                  <c:v>17.019545165380652</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.153194644315361</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.31807170176607613</c:v>
+                  <c:v>33.517807278913793</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,96 +514,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$O$16</c:f>
+              <c:f>Sheet1!$C$16:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-4.7499999999999991</c:v>
+                  <c:v>-5.5174999999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.274855905701624</c:v>
+                  <c:v>17.019545165380638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.033582288311202</c:v>
+                  <c:v>33.517807278913793</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.44962239153271</c:v>
+                  <c:v>35.517499999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2398190008976702</c:v>
+                  <c:v>23.961216948152522</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.7499999999999982</c:v>
+                  <c:v>7.4629548346193584</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-10.175480447459666</c:v>
+                  <c:v>-5.5174999999999974</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-14.763960944970705</c:v>
+                  <c:v>-12.980454834619355</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-20.347920841749197</c:v>
+                  <c:v>-18.443716948152513</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.210517352263626</c:v>
+                  <c:v>-24.482499999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-4.7500000000000107</c:v>
+                  <c:v>-28.000307278913805</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.274855905701592</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>28.033582288311202</c:v>
+                  <c:v>-22.537045165380654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$O$17</c:f>
+              <c:f>Sheet1!$C$17:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>27.25</c:v>
+                  <c:v>35.517499999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.188231549119298</c:v>
+                  <c:v>33.5178072789138</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.902031598544565</c:v>
+                  <c:v>17.019545165380645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-13.587693045106562</c:v>
+                  <c:v>-5.5174999999999974</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-21.252570102557293</c:v>
+                  <c:v>-22.537045165380633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-17.75</c:v>
+                  <c:v>-28.000307278913798</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-12.21753319775334</c:v>
+                  <c:v>-24.482500000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-8.0037331483280649</c:v>
+                  <c:v>-18.443716948152524</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.31807170176606725</c:v>
+                  <c:v>-12.980454834619367</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.153194644315327</c:v>
+                  <c:v>-5.5174999999999983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.249999999999993</c:v>
+                  <c:v>7.4629548346193664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.188231549119315</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.902031598544581</c:v>
+                  <c:v>23.961216948152511</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,96 +643,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$O$18</c:f>
+              <c:f>Sheet1!$C$18:$N$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-4.75</c:v>
+                  <c:v>-5.5175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2398190008976657</c:v>
+                  <c:v>7.4629548346193584</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.449622391532706</c:v>
+                  <c:v>23.961216948152515</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.033582288311202</c:v>
+                  <c:v>35.517499999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.274855905701628</c:v>
+                  <c:v>33.5178072789138</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.7499999999999956</c:v>
+                  <c:v>17.019545165380638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-19.210517352263622</c:v>
+                  <c:v>-5.5174999999999947</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-20.347920841749207</c:v>
+                  <c:v>-22.537045165380633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-14.763960944970712</c:v>
+                  <c:v>-28.000307278913802</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-10.175480447459664</c:v>
+                  <c:v>-24.482500000000009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-4.7499999999999982</c:v>
+                  <c:v>-18.44371694815252</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.2398190008976409</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.449622391532696</c:v>
+                  <c:v>-12.980454834619373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$O$19</c:f>
+              <c:f>Sheet1!$C$19:$N$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>17.75</c:v>
+                  <c:v>24.482500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.252570102557296</c:v>
+                  <c:v>28.000307278913798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.587693045106565</c:v>
+                  <c:v>22.537045165380643</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.9020315985445624</c:v>
+                  <c:v>5.5175000000000018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-24.188231549119294</c:v>
+                  <c:v>-17.019545165380631</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-27.25</c:v>
+                  <c:v>-33.5178072789138</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-15.153194644315343</c:v>
+                  <c:v>-35.517499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.31807170176607169</c:v>
+                  <c:v>-23.961216948152526</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0037331483280738</c:v>
+                  <c:v>-7.4629548346193761</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.217533197753339</c:v>
+                  <c:v>5.517500000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.749999999999993</c:v>
+                  <c:v>12.980454834619355</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.2525701025573</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.587693045106572</c:v>
+                  <c:v>18.443716948152513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,96 +772,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$O$20</c:f>
+              <c:f>Sheet1!$C$20:$N$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4.7499999999999991</c:v>
+                  <c:v>5.5174999999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.175480447459666</c:v>
+                  <c:v>12.980454834619358</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.763960944970705</c:v>
+                  <c:v>18.443716948152517</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.347920841749204</c:v>
+                  <c:v>24.482500000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.210517352263629</c:v>
+                  <c:v>28.000307278913798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7500000000000036</c:v>
+                  <c:v>22.53704516538064</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-16.274855905701621</c:v>
+                  <c:v>5.5175000000000045</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-28.033582288311202</c:v>
+                  <c:v>-17.019545165380627</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22.449622391532717</c:v>
+                  <c:v>-33.517807278913793</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-7.2398190008976755</c:v>
+                  <c:v>-35.517500000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.75</c:v>
+                  <c:v>-23.961216948152508</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.175480447459654</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14.763960944970705</c:v>
+                  <c:v>-7.4629548346193753</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$O$21</c:f>
+              <c:f>Sheet1!$C$21:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>17.75</c:v>
+                  <c:v>24.482500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.217533197753337</c:v>
+                  <c:v>18.44371694815252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0037331483280703</c:v>
+                  <c:v>12.980454834619362</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.31807170176606903</c:v>
+                  <c:v>5.517500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-15.153194644315334</c:v>
+                  <c:v>-7.4629548346193522</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-27.25</c:v>
+                  <c:v>-23.961216948152522</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-24.188231549119301</c:v>
+                  <c:v>-35.517499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.9020315985445748</c:v>
+                  <c:v>-33.517807278913807</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.587693045106558</c:v>
+                  <c:v>-17.019545165380663</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.2525701025573</c:v>
+                  <c:v>5.5174999999999876</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.750000000000007</c:v>
+                  <c:v>22.53704516538064</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.217533197753347</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.0037331483280667</c:v>
+                  <c:v>28.000307278913795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,96 +901,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$O$8</c:f>
+              <c:f>Sheet1!$C$8:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.225168176580645</c:v>
+                  <c:v>14.999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.398771616640953</c:v>
+                  <c:v>25.980762113533157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.398771616640957</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.225168176580649</c:v>
+                  <c:v>25.98076211353316</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.756584023544395E-15</c:v>
+                  <c:v>14.999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-13.225168176580643</c:v>
+                  <c:v>3.67544536472586E-15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-21.398771616640953</c:v>
+                  <c:v>-14.999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-21.398771616640957</c:v>
+                  <c:v>-25.980762113533153</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-13.225168176580651</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-5.51316804708879E-15</c:v>
+                  <c:v>-25.980762113533157</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.225168176580624</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21.398771616640953</c:v>
+                  <c:v>-15.000000000000014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$O$9</c:f>
+              <c:f>Sheet1!$C$9:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>22.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.202882373436317</c:v>
+                  <c:v>25.98076211353316</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9528823734363172</c:v>
+                  <c:v>15.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.9528823734363154</c:v>
+                  <c:v>1.83772268236293E-15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-18.202882373436314</c:v>
+                  <c:v>-14.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-22.5</c:v>
+                  <c:v>-25.98076211353316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.202882373436321</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-6.9528823734363199</c:v>
+                  <c:v>-25.980762113533164</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9528823734363128</c:v>
+                  <c:v>-15.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.202882373436314</c:v>
+                  <c:v>-5.51316804708879E-15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.5</c:v>
+                  <c:v>15.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.202882373436331</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.9528823734363243</c:v>
+                  <c:v>25.980762113533153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1620,16 +1709,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>6349</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>161923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>107155</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>83343</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1954,10 +2043,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1163DC21-E178-F645-AF41-DFB824044317}">
-  <dimension ref="B2:O21"/>
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1965,26 +2057,32 @@
     <col min="2" max="2" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>22.5</v>
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>11.035</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2024,11 +2122,8 @@
       <c r="N5" s="4">
         <v>12</v>
       </c>
-      <c r="O5" s="4">
-        <v>13</v>
-      </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2068,11 +2163,8 @@
       <c r="N6" s="2">
         <v>11</v>
       </c>
-      <c r="O6" s="2">
-        <v>12</v>
-      </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2081,169 +2173,157 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" ref="D7:O7" si="0">D6*2*PI()/$C$3</f>
-        <v>0.62831853071795862</v>
+        <f t="shared" ref="D7:N7" si="0">D6*2*PI()/$C$3</f>
+        <v>0.52359877559829882</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>1.2566370614359172</v>
+        <v>1.0471975511965976</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>1.8849555921538759</v>
+        <v>1.5707963267948966</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>2.5132741228718345</v>
+        <v>2.0943951023931953</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>3.1415926535897931</v>
+        <v>2.6179938779914944</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="0"/>
-        <v>3.7699111843077517</v>
+        <v>3.1415926535897931</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>4.3982297150257104</v>
+        <v>3.6651914291880918</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" si="0"/>
-        <v>5.026548245743669</v>
+        <v>4.1887902047863905</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" si="0"/>
-        <v>5.6548667764616276</v>
+        <v>4.7123889803846897</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>6.2831853071795862</v>
+        <v>5.2359877559829888</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="0"/>
-        <v>6.911503837897544</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="0"/>
-        <v>7.5398223686155035</v>
+        <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="13">
         <f>$C$2*SIN(C7)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="3">
-        <f t="shared" ref="D8:O8" si="1">$C$2*SIN(D7)</f>
-        <v>13.225168176580645</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="D8" s="13">
+        <f t="shared" ref="D8:N8" si="1">$C$2*SIN(D7)</f>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="E8" s="13">
         <f t="shared" si="1"/>
-        <v>21.398771616640953</v>
-      </c>
-      <c r="F8" s="3">
+        <v>25.980762113533157</v>
+      </c>
+      <c r="F8" s="13">
         <f t="shared" si="1"/>
-        <v>21.398771616640957</v>
-      </c>
-      <c r="G8" s="3">
+        <v>30</v>
+      </c>
+      <c r="G8" s="13">
         <f t="shared" si="1"/>
-        <v>13.225168176580649</v>
-      </c>
-      <c r="H8" s="3">
+        <v>25.98076211353316</v>
+      </c>
+      <c r="H8" s="13">
         <f t="shared" si="1"/>
-        <v>2.756584023544395E-15</v>
-      </c>
-      <c r="I8" s="3">
+        <v>14.999999999999998</v>
+      </c>
+      <c r="I8" s="13">
         <f t="shared" si="1"/>
-        <v>-13.225168176580643</v>
-      </c>
-      <c r="J8" s="3">
+        <v>3.67544536472586E-15</v>
+      </c>
+      <c r="J8" s="13">
         <f t="shared" si="1"/>
-        <v>-21.398771616640953</v>
-      </c>
-      <c r="K8" s="3">
+        <v>-14.999999999999991</v>
+      </c>
+      <c r="K8" s="13">
         <f t="shared" si="1"/>
-        <v>-21.398771616640957</v>
-      </c>
-      <c r="L8" s="3">
+        <v>-25.980762113533153</v>
+      </c>
+      <c r="L8" s="13">
         <f t="shared" si="1"/>
-        <v>-13.225168176580651</v>
-      </c>
-      <c r="M8" s="3">
+        <v>-30</v>
+      </c>
+      <c r="M8" s="13">
         <f t="shared" si="1"/>
-        <v>-5.51316804708879E-15</v>
-      </c>
-      <c r="N8" s="3">
+        <v>-25.980762113533157</v>
+      </c>
+      <c r="N8" s="13">
         <f t="shared" si="1"/>
-        <v>13.225168176580624</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="1"/>
-        <v>21.398771616640953</v>
+        <v>-15.000000000000014</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="14">
         <f>$C$2*COS(C7)</f>
-        <v>22.5</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" ref="D9:O9" si="2">$C$2*COS(D7)</f>
-        <v>18.202882373436317</v>
-      </c>
-      <c r="E9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" ref="D9:N9" si="2">$C$2*COS(D7)</f>
+        <v>25.98076211353316</v>
+      </c>
+      <c r="E9" s="14">
         <f t="shared" si="2"/>
-        <v>6.9528823734363172</v>
-      </c>
-      <c r="F9" s="3">
+        <v>15.000000000000004</v>
+      </c>
+      <c r="F9" s="14">
         <f t="shared" si="2"/>
-        <v>-6.9528823734363154</v>
-      </c>
-      <c r="G9" s="3">
+        <v>1.83772268236293E-15</v>
+      </c>
+      <c r="G9" s="14">
         <f t="shared" si="2"/>
-        <v>-18.202882373436314</v>
-      </c>
-      <c r="H9" s="3">
+        <v>-14.999999999999993</v>
+      </c>
+      <c r="H9" s="14">
         <f t="shared" si="2"/>
-        <v>-22.5</v>
-      </c>
-      <c r="I9" s="3">
+        <v>-25.98076211353316</v>
+      </c>
+      <c r="I9" s="14">
         <f t="shared" si="2"/>
-        <v>-18.202882373436321</v>
-      </c>
-      <c r="J9" s="3">
+        <v>-30</v>
+      </c>
+      <c r="J9" s="14">
         <f t="shared" si="2"/>
-        <v>-6.9528823734363199</v>
-      </c>
-      <c r="K9" s="3">
+        <v>-25.980762113533164</v>
+      </c>
+      <c r="K9" s="14">
         <f t="shared" si="2"/>
-        <v>6.9528823734363128</v>
-      </c>
-      <c r="L9" s="3">
+        <v>-15.000000000000014</v>
+      </c>
+      <c r="L9" s="14">
         <f t="shared" si="2"/>
-        <v>18.202882373436314</v>
-      </c>
-      <c r="M9" s="3">
+        <v>-5.51316804708879E-15</v>
+      </c>
+      <c r="M9" s="14">
         <f t="shared" si="2"/>
-        <v>22.5</v>
-      </c>
-      <c r="N9" s="3">
+        <v>15.000000000000004</v>
+      </c>
+      <c r="N9" s="14">
         <f t="shared" si="2"/>
-        <v>18.202882373436331</v>
-      </c>
-      <c r="O9" s="3">
-        <f t="shared" si="2"/>
-        <v>6.9528823734363243</v>
+        <v>25.980762113533153</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -2252,508 +2332,492 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" ref="D11:O11" si="3">2*D7</f>
-        <v>1.2566370614359172</v>
+        <f t="shared" ref="D11:N11" si="3">2*D7</f>
+        <v>1.0471975511965976</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="3"/>
-        <v>2.5132741228718345</v>
+        <v>2.0943951023931953</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="3"/>
-        <v>3.7699111843077517</v>
+        <v>3.1415926535897931</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="3"/>
-        <v>5.026548245743669</v>
+        <v>4.1887902047863905</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="3"/>
-        <v>6.2831853071795862</v>
+        <v>5.2359877559829888</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="3"/>
-        <v>7.5398223686155035</v>
+        <v>6.2831853071795862</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="3"/>
-        <v>8.7964594300514207</v>
+        <v>7.3303828583761836</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="3"/>
-        <v>10.053096491487338</v>
+        <v>8.3775804095727811</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" si="3"/>
-        <v>11.309733552923255</v>
+        <v>9.4247779607693793</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="3"/>
-        <v>12.566370614359172</v>
+        <v>10.471975511965978</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="3"/>
-        <v>13.823007675795088</v>
-      </c>
-      <c r="O11" s="3">
-        <f t="shared" si="3"/>
-        <v>15.079644737231007</v>
+        <v>11.519173063162574</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3">
-        <f>C$8+(9.5/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
-        <v>4.75</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" ref="D14:O14" si="4">D$8+(9.5/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
-        <v>19.210517352263626</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="C14" s="5">
+        <f>C$8+($E$2/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
+        <v>5.5175000000000001</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" ref="D14:N14" si="4">D$8+($E$2/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
+        <v>22.53704516538064</v>
+      </c>
+      <c r="E14" s="5">
         <f t="shared" si="4"/>
-        <v>20.3479208417492</v>
-      </c>
-      <c r="F14" s="3">
+        <v>28.000307278913798</v>
+      </c>
+      <c r="F14" s="5">
         <f t="shared" si="4"/>
-        <v>14.763960944970711</v>
-      </c>
-      <c r="G14" s="3">
+        <v>24.482500000000002</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="4"/>
-        <v>10.17548044745967</v>
-      </c>
-      <c r="H14" s="3">
+        <v>18.44371694815252</v>
+      </c>
+      <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>4.7500000000000009</v>
-      </c>
-      <c r="I14" s="3">
+        <v>12.980454834619358</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" si="4"/>
-        <v>-7.2398190008976631</v>
-      </c>
-      <c r="J14" s="3">
+        <v>5.5175000000000018</v>
+      </c>
+      <c r="J14" s="5">
         <f t="shared" si="4"/>
-        <v>-22.449622391532699</v>
-      </c>
-      <c r="K14" s="3">
+        <v>-7.4629548346193504</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="4"/>
-        <v>-28.033582288311202</v>
-      </c>
-      <c r="L14" s="3">
+        <v>-23.961216948152504</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="4"/>
-        <v>-16.274855905701639</v>
-      </c>
-      <c r="M14" s="3">
+        <v>-35.517499999999991</v>
+      </c>
+      <c r="M14" s="5">
         <f t="shared" si="4"/>
-        <v>4.7499999999999876</v>
-      </c>
-      <c r="N14" s="3">
+        <v>-33.517807278913793</v>
+      </c>
+      <c r="N14" s="5">
         <f t="shared" si="4"/>
-        <v>19.210517352263608</v>
-      </c>
-      <c r="O14" s="3">
-        <f t="shared" si="4"/>
-        <v>20.347920841749211</v>
+        <v>-17.019545165380656</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3">
-        <f>C$9+(9.5/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
-        <v>27.25</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" ref="D15:O15" si="5">D$9+(9.5/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
-        <v>15.153194644315338</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="C15" s="6">
+        <f>C$9+($E$2/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
+        <v>35.517499999999998</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" ref="D15:N15" si="5">D$9+($E$2/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
+        <v>23.961216948152522</v>
+      </c>
+      <c r="E15" s="6">
         <f t="shared" si="5"/>
-        <v>0.31807170176606991</v>
-      </c>
-      <c r="F15" s="3">
+        <v>7.4629548346193646</v>
+      </c>
+      <c r="F15" s="6">
         <f t="shared" si="5"/>
-        <v>-8.0037331483280685</v>
-      </c>
-      <c r="G15" s="3">
+        <v>-5.5174999999999983</v>
+      </c>
+      <c r="G15" s="6">
         <f t="shared" si="5"/>
-        <v>-12.217533197753335</v>
-      </c>
-      <c r="H15" s="3">
+        <v>-12.980454834619355</v>
+      </c>
+      <c r="H15" s="6">
         <f t="shared" si="5"/>
-        <v>-17.75</v>
-      </c>
-      <c r="I15" s="3">
+        <v>-18.44371694815252</v>
+      </c>
+      <c r="I15" s="6">
         <f t="shared" si="5"/>
-        <v>-21.2525701025573</v>
-      </c>
-      <c r="J15" s="3">
+        <v>-24.482499999999998</v>
+      </c>
+      <c r="J15" s="6">
         <f t="shared" si="5"/>
-        <v>-13.587693045106569</v>
-      </c>
-      <c r="K15" s="3">
+        <v>-28.000307278913802</v>
+      </c>
+      <c r="K15" s="6">
         <f t="shared" si="5"/>
-        <v>5.9020315985445517</v>
-      </c>
-      <c r="L15" s="3">
+        <v>-22.537045165380654</v>
+      </c>
+      <c r="L15" s="6">
         <f t="shared" si="5"/>
-        <v>24.188231549119287</v>
-      </c>
-      <c r="M15" s="3">
+        <v>-5.5175000000000116</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="5"/>
-        <v>27.250000000000007</v>
-      </c>
-      <c r="N15" s="3">
+        <v>17.019545165380652</v>
+      </c>
+      <c r="N15" s="6">
         <f t="shared" si="5"/>
-        <v>15.153194644315361</v>
-      </c>
-      <c r="O15" s="3">
-        <f t="shared" si="5"/>
-        <v>0.31807170176607613</v>
+        <v>33.517807278913793</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="3">
-        <f>C$8+(9.5/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
-        <v>-4.7499999999999991</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:O16" si="6">D$8+(9.5/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
-        <v>16.274855905701624</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="C16" s="7">
+        <f>C$8+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
+        <v>-5.5174999999999992</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" ref="D16:N16" si="6">D$8+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
+        <v>17.019545165380638</v>
+      </c>
+      <c r="E16" s="7">
         <f t="shared" si="6"/>
-        <v>28.033582288311202</v>
-      </c>
-      <c r="F16" s="3">
+        <v>33.517807278913793</v>
+      </c>
+      <c r="F16" s="7">
         <f t="shared" si="6"/>
-        <v>22.44962239153271</v>
-      </c>
-      <c r="G16" s="3">
+        <v>35.517499999999998</v>
+      </c>
+      <c r="G16" s="7">
         <f t="shared" si="6"/>
-        <v>7.2398190008976702</v>
-      </c>
-      <c r="H16" s="3">
+        <v>23.961216948152522</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="6"/>
-        <v>-4.7499999999999982</v>
-      </c>
-      <c r="I16" s="3">
+        <v>7.4629548346193584</v>
+      </c>
+      <c r="I16" s="7">
         <f t="shared" si="6"/>
-        <v>-10.175480447459666</v>
-      </c>
-      <c r="J16" s="3">
+        <v>-5.5174999999999974</v>
+      </c>
+      <c r="J16" s="7">
         <f t="shared" si="6"/>
-        <v>-14.763960944970705</v>
-      </c>
-      <c r="K16" s="3">
+        <v>-12.980454834619355</v>
+      </c>
+      <c r="K16" s="7">
         <f t="shared" si="6"/>
-        <v>-20.347920841749197</v>
-      </c>
-      <c r="L16" s="3">
+        <v>-18.443716948152513</v>
+      </c>
+      <c r="L16" s="7">
         <f t="shared" si="6"/>
-        <v>-19.210517352263626</v>
-      </c>
-      <c r="M16" s="3">
+        <v>-24.482499999999995</v>
+      </c>
+      <c r="M16" s="7">
         <f t="shared" si="6"/>
-        <v>-4.7500000000000107</v>
-      </c>
-      <c r="N16" s="3">
+        <v>-28.000307278913805</v>
+      </c>
+      <c r="N16" s="7">
         <f t="shared" si="6"/>
-        <v>16.274855905701592</v>
-      </c>
-      <c r="O16" s="3">
-        <f t="shared" si="6"/>
-        <v>28.033582288311202</v>
+        <v>-22.537045165380654</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3">
-        <f>C$9+(9.5/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
-        <v>27.25</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" ref="D17:O17" si="7">D$9+(9.5/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
-        <v>24.188231549119298</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="C17" s="8">
+        <f>C$9+($E$2/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
+        <v>35.517499999999998</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" ref="D17:N17" si="7">D$9+($E$2/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
+        <v>33.5178072789138</v>
+      </c>
+      <c r="E17" s="8">
         <f t="shared" si="7"/>
-        <v>5.902031598544565</v>
-      </c>
-      <c r="F17" s="3">
+        <v>17.019545165380645</v>
+      </c>
+      <c r="F17" s="8">
         <f t="shared" si="7"/>
-        <v>-13.587693045106562</v>
-      </c>
-      <c r="G17" s="3">
+        <v>-5.5174999999999974</v>
+      </c>
+      <c r="G17" s="8">
         <f t="shared" si="7"/>
-        <v>-21.252570102557293</v>
-      </c>
-      <c r="H17" s="3">
+        <v>-22.537045165380633</v>
+      </c>
+      <c r="H17" s="8">
         <f t="shared" si="7"/>
-        <v>-17.75</v>
-      </c>
-      <c r="I17" s="3">
+        <v>-28.000307278913798</v>
+      </c>
+      <c r="I17" s="8">
         <f t="shared" si="7"/>
-        <v>-12.21753319775334</v>
-      </c>
-      <c r="J17" s="3">
+        <v>-24.482500000000002</v>
+      </c>
+      <c r="J17" s="8">
         <f t="shared" si="7"/>
-        <v>-8.0037331483280649</v>
-      </c>
-      <c r="K17" s="3">
+        <v>-18.443716948152524</v>
+      </c>
+      <c r="K17" s="8">
         <f t="shared" si="7"/>
-        <v>0.31807170176606725</v>
-      </c>
-      <c r="L17" s="3">
+        <v>-12.980454834619367</v>
+      </c>
+      <c r="L17" s="8">
         <f t="shared" si="7"/>
-        <v>15.153194644315327</v>
-      </c>
-      <c r="M17" s="3">
+        <v>-5.5174999999999983</v>
+      </c>
+      <c r="M17" s="8">
         <f t="shared" si="7"/>
-        <v>27.249999999999993</v>
-      </c>
-      <c r="N17" s="3">
+        <v>7.4629548346193664</v>
+      </c>
+      <c r="N17" s="8">
         <f t="shared" si="7"/>
-        <v>24.188231549119315</v>
-      </c>
-      <c r="O17" s="3">
-        <f t="shared" si="7"/>
-        <v>5.902031598544581</v>
+        <v>23.961216948152511</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3">
-        <f>C$8+(9.5/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
-        <v>-4.75</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" ref="D18:O18" si="8">D$8+(9.5/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
-        <v>7.2398190008976657</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="C18" s="9">
+        <f>C$8+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
+        <v>-5.5175000000000001</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" ref="D18:N18" si="8">D$8+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
+        <v>7.4629548346193584</v>
+      </c>
+      <c r="E18" s="9">
         <f t="shared" si="8"/>
-        <v>22.449622391532706</v>
-      </c>
-      <c r="F18" s="3">
+        <v>23.961216948152515</v>
+      </c>
+      <c r="F18" s="9">
         <f t="shared" si="8"/>
-        <v>28.033582288311202</v>
-      </c>
-      <c r="G18" s="3">
+        <v>35.517499999999998</v>
+      </c>
+      <c r="G18" s="9">
         <f t="shared" si="8"/>
-        <v>16.274855905701628</v>
-      </c>
-      <c r="H18" s="3">
+        <v>33.5178072789138</v>
+      </c>
+      <c r="H18" s="9">
         <f t="shared" si="8"/>
-        <v>-4.7499999999999956</v>
-      </c>
-      <c r="I18" s="3">
+        <v>17.019545165380638</v>
+      </c>
+      <c r="I18" s="9">
         <f t="shared" si="8"/>
-        <v>-19.210517352263622</v>
-      </c>
-      <c r="J18" s="3">
+        <v>-5.5174999999999947</v>
+      </c>
+      <c r="J18" s="9">
         <f t="shared" si="8"/>
-        <v>-20.347920841749207</v>
-      </c>
-      <c r="K18" s="3">
+        <v>-22.537045165380633</v>
+      </c>
+      <c r="K18" s="9">
         <f t="shared" si="8"/>
-        <v>-14.763960944970712</v>
-      </c>
-      <c r="L18" s="3">
+        <v>-28.000307278913802</v>
+      </c>
+      <c r="L18" s="9">
         <f t="shared" si="8"/>
-        <v>-10.175480447459664</v>
-      </c>
-      <c r="M18" s="3">
+        <v>-24.482500000000009</v>
+      </c>
+      <c r="M18" s="9">
         <f t="shared" si="8"/>
-        <v>-4.7499999999999982</v>
-      </c>
-      <c r="N18" s="3">
+        <v>-18.44371694815252</v>
+      </c>
+      <c r="N18" s="9">
         <f t="shared" si="8"/>
-        <v>7.2398190008976409</v>
-      </c>
-      <c r="O18" s="3">
-        <f t="shared" si="8"/>
-        <v>22.449622391532696</v>
+        <v>-12.980454834619373</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="3">
-        <f>C$9+(9.5/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
-        <v>17.75</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" ref="D19:O19" si="9">D$9+(9.5/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
-        <v>21.252570102557296</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="C19" s="10">
+        <f>C$9+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
+        <v>24.482500000000002</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" ref="D19:N19" si="9">D$9+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
+        <v>28.000307278913798</v>
+      </c>
+      <c r="E19" s="10">
         <f t="shared" si="9"/>
-        <v>13.587693045106565</v>
-      </c>
-      <c r="F19" s="3">
+        <v>22.537045165380643</v>
+      </c>
+      <c r="F19" s="10">
         <f t="shared" si="9"/>
-        <v>-5.9020315985445624</v>
-      </c>
-      <c r="G19" s="3">
+        <v>5.5175000000000018</v>
+      </c>
+      <c r="G19" s="10">
         <f t="shared" si="9"/>
-        <v>-24.188231549119294</v>
-      </c>
-      <c r="H19" s="3">
+        <v>-17.019545165380631</v>
+      </c>
+      <c r="H19" s="10">
         <f t="shared" si="9"/>
-        <v>-27.25</v>
-      </c>
-      <c r="I19" s="3">
+        <v>-33.5178072789138</v>
+      </c>
+      <c r="I19" s="10">
         <f t="shared" si="9"/>
-        <v>-15.153194644315343</v>
-      </c>
-      <c r="J19" s="3">
+        <v>-35.517499999999998</v>
+      </c>
+      <c r="J19" s="10">
         <f t="shared" si="9"/>
-        <v>-0.31807170176607169</v>
-      </c>
-      <c r="K19" s="3">
+        <v>-23.961216948152526</v>
+      </c>
+      <c r="K19" s="10">
         <f t="shared" si="9"/>
-        <v>8.0037331483280738</v>
-      </c>
-      <c r="L19" s="3">
+        <v>-7.4629548346193761</v>
+      </c>
+      <c r="L19" s="10">
         <f t="shared" si="9"/>
-        <v>12.217533197753339</v>
-      </c>
-      <c r="M19" s="3">
+        <v>5.517500000000001</v>
+      </c>
+      <c r="M19" s="10">
         <f t="shared" si="9"/>
-        <v>17.749999999999993</v>
-      </c>
-      <c r="N19" s="3">
+        <v>12.980454834619355</v>
+      </c>
+      <c r="N19" s="10">
         <f t="shared" si="9"/>
-        <v>21.2525701025573</v>
-      </c>
-      <c r="O19" s="3">
-        <f t="shared" si="9"/>
-        <v>13.587693045106572</v>
+        <v>18.443716948152513</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3">
-        <f>C$8+(9.5/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
-        <v>4.7499999999999991</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" ref="D20:O20" si="10">D$8+(9.5/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
-        <v>10.175480447459666</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="C20" s="11">
+        <f>C$8+($E$2/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
+        <v>5.5174999999999992</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" ref="D20:N20" si="10">D$8+($E$2/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
+        <v>12.980454834619358</v>
+      </c>
+      <c r="E20" s="11">
         <f t="shared" si="10"/>
-        <v>14.763960944970705</v>
-      </c>
-      <c r="F20" s="3">
+        <v>18.443716948152517</v>
+      </c>
+      <c r="F20" s="11">
         <f t="shared" si="10"/>
-        <v>20.347920841749204</v>
-      </c>
-      <c r="G20" s="3">
+        <v>24.482500000000002</v>
+      </c>
+      <c r="G20" s="11">
         <f t="shared" si="10"/>
-        <v>19.210517352263629</v>
-      </c>
-      <c r="H20" s="3">
+        <v>28.000307278913798</v>
+      </c>
+      <c r="H20" s="11">
         <f t="shared" si="10"/>
-        <v>4.7500000000000036</v>
-      </c>
-      <c r="I20" s="3">
+        <v>22.53704516538064</v>
+      </c>
+      <c r="I20" s="11">
         <f t="shared" si="10"/>
-        <v>-16.274855905701621</v>
-      </c>
-      <c r="J20" s="3">
+        <v>5.5175000000000045</v>
+      </c>
+      <c r="J20" s="11">
         <f t="shared" si="10"/>
-        <v>-28.033582288311202</v>
-      </c>
-      <c r="K20" s="3">
+        <v>-17.019545165380627</v>
+      </c>
+      <c r="K20" s="11">
         <f t="shared" si="10"/>
-        <v>-22.449622391532717</v>
-      </c>
-      <c r="L20" s="3">
+        <v>-33.517807278913793</v>
+      </c>
+      <c r="L20" s="11">
         <f t="shared" si="10"/>
-        <v>-7.2398190008976755</v>
-      </c>
-      <c r="M20" s="3">
+        <v>-35.517500000000005</v>
+      </c>
+      <c r="M20" s="11">
         <f t="shared" si="10"/>
-        <v>4.75</v>
-      </c>
-      <c r="N20" s="3">
+        <v>-23.961216948152508</v>
+      </c>
+      <c r="N20" s="11">
         <f t="shared" si="10"/>
-        <v>10.175480447459654</v>
-      </c>
-      <c r="O20" s="3">
-        <f t="shared" si="10"/>
-        <v>14.763960944970705</v>
+        <v>-7.4629548346193753</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3">
-        <f>C$9+(9.5/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
-        <v>17.75</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" ref="D21:O21" si="11">D$9+(9.5/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
-        <v>12.217533197753337</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="C21" s="12">
+        <f>C$9+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
+        <v>24.482500000000002</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" ref="D21:N21" si="11">D$9+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
+        <v>18.44371694815252</v>
+      </c>
+      <c r="E21" s="12">
         <f t="shared" si="11"/>
-        <v>8.0037331483280703</v>
-      </c>
-      <c r="F21" s="3">
+        <v>12.980454834619362</v>
+      </c>
+      <c r="F21" s="12">
         <f t="shared" si="11"/>
-        <v>-0.31807170176606903</v>
-      </c>
-      <c r="G21" s="3">
+        <v>5.517500000000001</v>
+      </c>
+      <c r="G21" s="12">
         <f t="shared" si="11"/>
-        <v>-15.153194644315334</v>
-      </c>
-      <c r="H21" s="3">
+        <v>-7.4629548346193522</v>
+      </c>
+      <c r="H21" s="12">
         <f t="shared" si="11"/>
-        <v>-27.25</v>
-      </c>
-      <c r="I21" s="3">
+        <v>-23.961216948152522</v>
+      </c>
+      <c r="I21" s="12">
         <f t="shared" si="11"/>
-        <v>-24.188231549119301</v>
-      </c>
-      <c r="J21" s="3">
+        <v>-35.517499999999998</v>
+      </c>
+      <c r="J21" s="12">
         <f t="shared" si="11"/>
-        <v>-5.9020315985445748</v>
-      </c>
-      <c r="K21" s="3">
+        <v>-33.517807278913807</v>
+      </c>
+      <c r="K21" s="12">
         <f t="shared" si="11"/>
-        <v>13.587693045106558</v>
-      </c>
-      <c r="L21" s="3">
+        <v>-17.019545165380663</v>
+      </c>
+      <c r="L21" s="12">
         <f t="shared" si="11"/>
-        <v>21.2525701025573</v>
-      </c>
-      <c r="M21" s="3">
+        <v>5.5174999999999876</v>
+      </c>
+      <c r="M21" s="12">
         <f t="shared" si="11"/>
-        <v>17.750000000000007</v>
-      </c>
-      <c r="N21" s="3">
+        <v>22.53704516538064</v>
+      </c>
+      <c r="N21" s="12">
         <f t="shared" si="11"/>
-        <v>12.217533197753347</v>
-      </c>
-      <c r="O21" s="3">
-        <f t="shared" si="11"/>
-        <v>8.0037331483280667</v>
+        <v>28.000307278913795</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <f>E2/2</f>
+        <v>5.5175000000000001</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update HalbachPositions (version 1).xlsx
</commit_message>
<xml_diff>
--- a/HalbachPositions (version 1).xlsx
+++ b/HalbachPositions (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steph\Documents\GitHub\Hallbach_cylinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD22E52-9BA8-44C2-B5FB-304753A8AC88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78057C7-E34B-4152-BFD6-7EA53CB6217D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5A3979A9-2DE4-234A-B973-A6AC692A53E8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t># of magnets</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Ring height</t>
-  </si>
-  <si>
-    <t>≈5.5</t>
   </si>
 </sst>
 </file>
@@ -342,8 +339,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.3970030474244572E-2"/>
-          <c:y val="6.513444610423022E-2"/>
+          <c:x val="3.9525584787753747E-2"/>
+          <c:y val="5.7463764545758349E-2"/>
           <c:w val="0.93947598285519696"/>
           <c:h val="0.92522003684530818"/>
         </c:manualLayout>
@@ -390,40 +387,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.5175000000000001</c:v>
+                  <c:v>5.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.53704516538064</c:v>
+                  <c:v>19.569181464584467</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.000307278913798</c:v>
+                  <c:v>23.544816559195436</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.482500000000002</c:v>
+                  <c:v>19.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.44371694815252</c:v>
+                  <c:v>14.581453630026498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.980454834619358</c:v>
+                  <c:v>10.60581853541553</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5175000000000018</c:v>
+                  <c:v>5.1750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7.4629548346193504</c:v>
+                  <c:v>-5.430818535415523</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-23.961216948152504</c:v>
+                  <c:v>-19.756453630026481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-35.517499999999991</c:v>
+                  <c:v>-30.174999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-33.517807278913793</c:v>
+                  <c:v>-28.719816559195433</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-17.019545165380656</c:v>
+                  <c:v>-14.394181464584481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,40 +432,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>35.517499999999998</c:v>
+                  <c:v>30.174999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.961216948152522</c:v>
+                  <c:v>19.756453630026499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4629548346193646</c:v>
+                  <c:v>5.4308185354155354</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.5174999999999983</c:v>
+                  <c:v>-5.174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-12.980454834619355</c:v>
+                  <c:v>-10.605818535415528</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-18.44371694815252</c:v>
+                  <c:v>-14.5814536300265</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-24.482499999999998</c:v>
+                  <c:v>-19.824999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-28.000307278913802</c:v>
+                  <c:v>-23.544816559195436</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22.537045165380654</c:v>
+                  <c:v>-19.569181464584478</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.5175000000000116</c:v>
+                  <c:v>-5.1750000000000096</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.019545165380652</c:v>
+                  <c:v>14.394181464584481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33.517807278913793</c:v>
+                  <c:v>28.719816559195426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -519,40 +516,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-5.5174999999999992</c:v>
+                  <c:v>-5.1749999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.019545165380638</c:v>
+                  <c:v>14.394181464584467</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.517807278913793</c:v>
+                  <c:v>28.719816559195433</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.517499999999998</c:v>
+                  <c:v>30.175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.961216948152522</c:v>
+                  <c:v>19.756453630026503</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4629548346193584</c:v>
+                  <c:v>5.4308185354155292</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.5174999999999974</c:v>
+                  <c:v>-5.174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-12.980454834619355</c:v>
+                  <c:v>-10.605818535415526</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-18.443716948152513</c:v>
+                  <c:v>-14.581453630026491</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-24.482499999999995</c:v>
+                  <c:v>-19.824999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-28.000307278913805</c:v>
+                  <c:v>-23.544816559195443</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-22.537045165380654</c:v>
+                  <c:v>-19.569181464584478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,40 +561,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>35.517499999999998</c:v>
+                  <c:v>30.175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.5178072789138</c:v>
+                  <c:v>28.719816559195436</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.019545165380645</c:v>
+                  <c:v>14.394181464584475</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.5174999999999974</c:v>
+                  <c:v>-5.1749999999999972</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-22.537045165380633</c:v>
+                  <c:v>-19.569181464584464</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-28.000307278913798</c:v>
+                  <c:v>-23.544816559195439</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-24.482500000000002</c:v>
+                  <c:v>-19.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18.443716948152524</c:v>
+                  <c:v>-14.581453630026498</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-12.980454834619367</c:v>
+                  <c:v>-10.605818535415535</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.5174999999999983</c:v>
+                  <c:v>-5.1749999999999972</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4629548346193664</c:v>
+                  <c:v>5.4308185354155372</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.961216948152511</c:v>
+                  <c:v>19.756453630026488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,40 +645,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-5.5175000000000001</c:v>
+                  <c:v>-5.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4629548346193584</c:v>
+                  <c:v>5.4308185354155292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.961216948152515</c:v>
+                  <c:v>19.756453630026495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.517499999999998</c:v>
+                  <c:v>30.174999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.5178072789138</c:v>
+                  <c:v>28.71981655919544</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.019545165380638</c:v>
+                  <c:v>14.394181464584467</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.5174999999999947</c:v>
+                  <c:v>-5.1749999999999954</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-22.537045165380633</c:v>
+                  <c:v>-19.569181464584464</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-28.000307278913802</c:v>
+                  <c:v>-23.544816559195436</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-24.482500000000009</c:v>
+                  <c:v>-19.825000000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-18.44371694815252</c:v>
+                  <c:v>-14.581453630026498</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-12.980454834619373</c:v>
+                  <c:v>-10.605818535415541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -693,40 +690,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>24.482500000000002</c:v>
+                  <c:v>19.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.000307278913798</c:v>
+                  <c:v>23.544816559195439</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.537045165380643</c:v>
+                  <c:v>19.569181464584471</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5175000000000018</c:v>
+                  <c:v>5.1750000000000016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-17.019545165380631</c:v>
+                  <c:v>-14.394181464584461</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-33.5178072789138</c:v>
+                  <c:v>-28.719816559195436</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-35.517499999999998</c:v>
+                  <c:v>-30.175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-23.961216948152526</c:v>
+                  <c:v>-19.756453630026503</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-7.4629548346193761</c:v>
+                  <c:v>-5.4308185354155434</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.517500000000001</c:v>
+                  <c:v>5.1750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.980454834619355</c:v>
+                  <c:v>10.605818535415526</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.443716948152513</c:v>
+                  <c:v>14.581453630026491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,40 +774,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.5174999999999992</c:v>
+                  <c:v>5.1749999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.980454834619358</c:v>
+                  <c:v>10.60581853541553</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.443716948152517</c:v>
+                  <c:v>14.581453630026498</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.482500000000002</c:v>
+                  <c:v>19.824999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.000307278913798</c:v>
+                  <c:v>23.544816559195436</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.53704516538064</c:v>
+                  <c:v>19.569181464584467</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5175000000000045</c:v>
+                  <c:v>5.1750000000000034</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-17.019545165380627</c:v>
+                  <c:v>-14.394181464584459</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-33.517807278913793</c:v>
+                  <c:v>-28.719816559195426</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-35.517500000000005</c:v>
+                  <c:v>-30.175000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-23.961216948152508</c:v>
+                  <c:v>-19.756453630026488</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-7.4629548346193753</c:v>
+                  <c:v>-5.4308185354155425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -822,40 +819,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>24.482500000000002</c:v>
+                  <c:v>19.824999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.44371694815252</c:v>
+                  <c:v>14.5814536300265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.980454834619362</c:v>
+                  <c:v>10.605818535415532</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.517500000000001</c:v>
+                  <c:v>5.1750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.4629548346193522</c:v>
+                  <c:v>-5.4308185354155247</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-23.961216948152522</c:v>
+                  <c:v>-19.756453630026499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-35.517499999999998</c:v>
+                  <c:v>-30.174999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-33.517807278913807</c:v>
+                  <c:v>-28.71981655919544</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-17.019545165380663</c:v>
+                  <c:v>-14.394181464584486</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5174999999999876</c:v>
+                  <c:v>5.1749999999999883</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.53704516538064</c:v>
+                  <c:v>19.569181464584471</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.000307278913795</c:v>
+                  <c:v>23.544816559195429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,37 +906,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.999999999999998</c:v>
+                  <c:v>12.499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.980762113533157</c:v>
+                  <c:v>21.650635094610966</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.98076211353316</c:v>
+                  <c:v>21.650635094610969</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.999999999999998</c:v>
+                  <c:v>12.499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.67544536472586E-15</c:v>
+                  <c:v>3.06287113727155E-15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-14.999999999999991</c:v>
+                  <c:v>-12.499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-25.980762113533153</c:v>
+                  <c:v>-21.650635094610958</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-30</c:v>
+                  <c:v>-25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-25.980762113533157</c:v>
+                  <c:v>-21.650635094610966</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-15.000000000000014</c:v>
+                  <c:v>-12.500000000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,40 +948,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.98076211353316</c:v>
+                  <c:v>21.650635094610969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.000000000000004</c:v>
+                  <c:v>12.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.83772268236293E-15</c:v>
+                  <c:v>1.531435568635775E-15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-14.999999999999993</c:v>
+                  <c:v>-12.499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-25.98076211353316</c:v>
+                  <c:v>-21.650635094610969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-30</c:v>
+                  <c:v>-25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-25.980762113533164</c:v>
+                  <c:v>-21.650635094610969</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-15.000000000000014</c:v>
+                  <c:v>-12.500000000000011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.51316804708879E-15</c:v>
+                  <c:v>-4.594306705907325E-15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.000000000000004</c:v>
+                  <c:v>12.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.980762113533153</c:v>
+                  <c:v>21.650635094610958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1710,15 +1707,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>6349</xdr:colOff>
+      <xdr:colOff>309562</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>161923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>83343</xdr:rowOff>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>130970</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2048,8 +2045,8 @@
   </sheetPr>
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2062,13 +2059,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2">
-        <v>11.035</v>
+        <v>10.35</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -2227,47 +2224,47 @@
       </c>
       <c r="D8" s="13">
         <f t="shared" ref="D8:N8" si="1">$C$2*SIN(D7)</f>
-        <v>14.999999999999998</v>
+        <v>12.499999999999998</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="1"/>
-        <v>25.980762113533157</v>
+        <v>21.650635094610966</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="1"/>
-        <v>25.98076211353316</v>
+        <v>21.650635094610969</v>
       </c>
       <c r="H8" s="13">
         <f t="shared" si="1"/>
-        <v>14.999999999999998</v>
+        <v>12.499999999999998</v>
       </c>
       <c r="I8" s="13">
         <f t="shared" si="1"/>
-        <v>3.67544536472586E-15</v>
+        <v>3.06287113727155E-15</v>
       </c>
       <c r="J8" s="13">
         <f t="shared" si="1"/>
-        <v>-14.999999999999991</v>
+        <v>-12.499999999999993</v>
       </c>
       <c r="K8" s="13">
         <f t="shared" si="1"/>
-        <v>-25.980762113533153</v>
+        <v>-21.650635094610958</v>
       </c>
       <c r="L8" s="13">
         <f t="shared" si="1"/>
-        <v>-30</v>
+        <v>-25</v>
       </c>
       <c r="M8" s="13">
         <f t="shared" si="1"/>
-        <v>-25.980762113533157</v>
+        <v>-21.650635094610966</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="1"/>
-        <v>-15.000000000000014</v>
+        <v>-12.500000000000011</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
@@ -2276,51 +2273,51 @@
       </c>
       <c r="C9" s="14">
         <f>$C$2*COS(C7)</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="14">
         <f t="shared" ref="D9:N9" si="2">$C$2*COS(D7)</f>
-        <v>25.98076211353316</v>
+        <v>21.650635094610969</v>
       </c>
       <c r="E9" s="14">
         <f t="shared" si="2"/>
-        <v>15.000000000000004</v>
+        <v>12.500000000000004</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="2"/>
-        <v>1.83772268236293E-15</v>
+        <v>1.531435568635775E-15</v>
       </c>
       <c r="G9" s="14">
         <f t="shared" si="2"/>
-        <v>-14.999999999999993</v>
+        <v>-12.499999999999995</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="2"/>
-        <v>-25.98076211353316</v>
+        <v>-21.650635094610969</v>
       </c>
       <c r="I9" s="14">
         <f t="shared" si="2"/>
-        <v>-30</v>
+        <v>-25</v>
       </c>
       <c r="J9" s="14">
         <f t="shared" si="2"/>
-        <v>-25.980762113533164</v>
+        <v>-21.650635094610969</v>
       </c>
       <c r="K9" s="14">
         <f t="shared" si="2"/>
-        <v>-15.000000000000014</v>
+        <v>-12.500000000000011</v>
       </c>
       <c r="L9" s="14">
         <f t="shared" si="2"/>
-        <v>-5.51316804708879E-15</v>
+        <v>-4.594306705907325E-15</v>
       </c>
       <c r="M9" s="14">
         <f t="shared" si="2"/>
-        <v>15.000000000000004</v>
+        <v>12.500000000000004</v>
       </c>
       <c r="N9" s="14">
         <f t="shared" si="2"/>
-        <v>25.980762113533153</v>
+        <v>21.650635094610958</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -2382,51 +2379,51 @@
       </c>
       <c r="C14" s="5">
         <f>C$8+($E$2/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
-        <v>5.5175000000000001</v>
+        <v>5.1749999999999998</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" ref="D14:N14" si="4">D$8+($E$2/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
-        <v>22.53704516538064</v>
+        <v>19.569181464584467</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="4"/>
-        <v>28.000307278913798</v>
+        <v>23.544816559195436</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="4"/>
-        <v>24.482500000000002</v>
+        <v>19.825000000000003</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="4"/>
-        <v>18.44371694815252</v>
+        <v>14.581453630026498</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>12.980454834619358</v>
+        <v>10.60581853541553</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="4"/>
-        <v>5.5175000000000018</v>
+        <v>5.1750000000000007</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="4"/>
-        <v>-7.4629548346193504</v>
+        <v>-5.430818535415523</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="4"/>
-        <v>-23.961216948152504</v>
+        <v>-19.756453630026481</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="4"/>
-        <v>-35.517499999999991</v>
+        <v>-30.174999999999994</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="4"/>
-        <v>-33.517807278913793</v>
+        <v>-28.719816559195433</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="4"/>
-        <v>-17.019545165380656</v>
+        <v>-14.394181464584481</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -2435,51 +2432,51 @@
       </c>
       <c r="C15" s="6">
         <f>C$9+($E$2/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
-        <v>35.517499999999998</v>
+        <v>30.174999999999997</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" ref="D15:N15" si="5">D$9+($E$2/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
-        <v>23.961216948152522</v>
+        <v>19.756453630026499</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="5"/>
-        <v>7.4629548346193646</v>
+        <v>5.4308185354155354</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" si="5"/>
-        <v>-5.5174999999999983</v>
+        <v>-5.174999999999998</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" si="5"/>
-        <v>-12.980454834619355</v>
+        <v>-10.605818535415528</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="5"/>
-        <v>-18.44371694815252</v>
+        <v>-14.5814536300265</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="5"/>
-        <v>-24.482499999999998</v>
+        <v>-19.824999999999999</v>
       </c>
       <c r="J15" s="6">
         <f t="shared" si="5"/>
-        <v>-28.000307278913802</v>
+        <v>-23.544816559195436</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="5"/>
-        <v>-22.537045165380654</v>
+        <v>-19.569181464584478</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="5"/>
-        <v>-5.5175000000000116</v>
+        <v>-5.1750000000000096</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="5"/>
-        <v>17.019545165380652</v>
+        <v>14.394181464584481</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="5"/>
-        <v>33.517807278913793</v>
+        <v>28.719816559195426</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -2488,51 +2485,51 @@
       </c>
       <c r="C16" s="7">
         <f>C$8+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
-        <v>-5.5174999999999992</v>
+        <v>-5.1749999999999989</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" ref="D16:N16" si="6">D$8+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
-        <v>17.019545165380638</v>
+        <v>14.394181464584467</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="6"/>
-        <v>33.517807278913793</v>
+        <v>28.719816559195433</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="6"/>
-        <v>35.517499999999998</v>
+        <v>30.175000000000001</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="6"/>
-        <v>23.961216948152522</v>
+        <v>19.756453630026503</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="6"/>
-        <v>7.4629548346193584</v>
+        <v>5.4308185354155292</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" si="6"/>
-        <v>-5.5174999999999974</v>
+        <v>-5.174999999999998</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" si="6"/>
-        <v>-12.980454834619355</v>
+        <v>-10.605818535415526</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="6"/>
-        <v>-18.443716948152513</v>
+        <v>-14.581453630026491</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="6"/>
-        <v>-24.482499999999995</v>
+        <v>-19.824999999999996</v>
       </c>
       <c r="M16" s="7">
         <f t="shared" si="6"/>
-        <v>-28.000307278913805</v>
+        <v>-23.544816559195443</v>
       </c>
       <c r="N16" s="7">
         <f t="shared" si="6"/>
-        <v>-22.537045165380654</v>
+        <v>-19.569181464584478</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -2541,51 +2538,51 @@
       </c>
       <c r="C17" s="8">
         <f>C$9+($E$2/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
-        <v>35.517499999999998</v>
+        <v>30.175000000000001</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" ref="D17:N17" si="7">D$9+($E$2/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
-        <v>33.5178072789138</v>
+        <v>28.719816559195436</v>
       </c>
       <c r="E17" s="8">
         <f t="shared" si="7"/>
-        <v>17.019545165380645</v>
+        <v>14.394181464584475</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="7"/>
-        <v>-5.5174999999999974</v>
+        <v>-5.1749999999999972</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="7"/>
-        <v>-22.537045165380633</v>
+        <v>-19.569181464584464</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="7"/>
-        <v>-28.000307278913798</v>
+        <v>-23.544816559195439</v>
       </c>
       <c r="I17" s="8">
         <f t="shared" si="7"/>
-        <v>-24.482500000000002</v>
+        <v>-19.825000000000003</v>
       </c>
       <c r="J17" s="8">
         <f t="shared" si="7"/>
-        <v>-18.443716948152524</v>
+        <v>-14.581453630026498</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="7"/>
-        <v>-12.980454834619367</v>
+        <v>-10.605818535415535</v>
       </c>
       <c r="L17" s="8">
         <f t="shared" si="7"/>
-        <v>-5.5174999999999983</v>
+        <v>-5.1749999999999972</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" si="7"/>
-        <v>7.4629548346193664</v>
+        <v>5.4308185354155372</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" si="7"/>
-        <v>23.961216948152511</v>
+        <v>19.756453630026488</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -2594,51 +2591,51 @@
       </c>
       <c r="C18" s="9">
         <f>C$8+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
-        <v>-5.5175000000000001</v>
+        <v>-5.1749999999999998</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" ref="D18:N18" si="8">D$8+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
-        <v>7.4629548346193584</v>
+        <v>5.4308185354155292</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="8"/>
-        <v>23.961216948152515</v>
+        <v>19.756453630026495</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="8"/>
-        <v>35.517499999999998</v>
+        <v>30.174999999999997</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="8"/>
-        <v>33.5178072789138</v>
+        <v>28.71981655919544</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" si="8"/>
-        <v>17.019545165380638</v>
+        <v>14.394181464584467</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="8"/>
-        <v>-5.5174999999999947</v>
+        <v>-5.1749999999999954</v>
       </c>
       <c r="J18" s="9">
         <f t="shared" si="8"/>
-        <v>-22.537045165380633</v>
+        <v>-19.569181464584464</v>
       </c>
       <c r="K18" s="9">
         <f t="shared" si="8"/>
-        <v>-28.000307278913802</v>
+        <v>-23.544816559195436</v>
       </c>
       <c r="L18" s="9">
         <f t="shared" si="8"/>
-        <v>-24.482500000000009</v>
+        <v>-19.825000000000006</v>
       </c>
       <c r="M18" s="9">
         <f t="shared" si="8"/>
-        <v>-18.44371694815252</v>
+        <v>-14.581453630026498</v>
       </c>
       <c r="N18" s="9">
         <f t="shared" si="8"/>
-        <v>-12.980454834619373</v>
+        <v>-10.605818535415541</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -2647,51 +2644,51 @@
       </c>
       <c r="C19" s="10">
         <f>C$9+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
-        <v>24.482500000000002</v>
+        <v>19.825000000000003</v>
       </c>
       <c r="D19" s="10">
         <f t="shared" ref="D19:N19" si="9">D$9+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
-        <v>28.000307278913798</v>
+        <v>23.544816559195439</v>
       </c>
       <c r="E19" s="10">
         <f t="shared" si="9"/>
-        <v>22.537045165380643</v>
+        <v>19.569181464584471</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="9"/>
-        <v>5.5175000000000018</v>
+        <v>5.1750000000000016</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" si="9"/>
-        <v>-17.019545165380631</v>
+        <v>-14.394181464584461</v>
       </c>
       <c r="H19" s="10">
         <f t="shared" si="9"/>
-        <v>-33.5178072789138</v>
+        <v>-28.719816559195436</v>
       </c>
       <c r="I19" s="10">
         <f t="shared" si="9"/>
-        <v>-35.517499999999998</v>
+        <v>-30.175000000000001</v>
       </c>
       <c r="J19" s="10">
         <f t="shared" si="9"/>
-        <v>-23.961216948152526</v>
+        <v>-19.756453630026503</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="9"/>
-        <v>-7.4629548346193761</v>
+        <v>-5.4308185354155434</v>
       </c>
       <c r="L19" s="10">
         <f t="shared" si="9"/>
-        <v>5.517500000000001</v>
+        <v>5.1750000000000007</v>
       </c>
       <c r="M19" s="10">
         <f t="shared" si="9"/>
-        <v>12.980454834619355</v>
+        <v>10.605818535415526</v>
       </c>
       <c r="N19" s="10">
         <f t="shared" si="9"/>
-        <v>18.443716948152513</v>
+        <v>14.581453630026491</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -2700,51 +2697,51 @@
       </c>
       <c r="C20" s="11">
         <f>C$8+($E$2/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
-        <v>5.5174999999999992</v>
+        <v>5.1749999999999989</v>
       </c>
       <c r="D20" s="11">
         <f t="shared" ref="D20:N20" si="10">D$8+($E$2/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
-        <v>12.980454834619358</v>
+        <v>10.60581853541553</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="10"/>
-        <v>18.443716948152517</v>
+        <v>14.581453630026498</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="10"/>
-        <v>24.482500000000002</v>
+        <v>19.824999999999999</v>
       </c>
       <c r="G20" s="11">
         <f t="shared" si="10"/>
-        <v>28.000307278913798</v>
+        <v>23.544816559195436</v>
       </c>
       <c r="H20" s="11">
         <f t="shared" si="10"/>
-        <v>22.53704516538064</v>
+        <v>19.569181464584467</v>
       </c>
       <c r="I20" s="11">
         <f t="shared" si="10"/>
-        <v>5.5175000000000045</v>
+        <v>5.1750000000000034</v>
       </c>
       <c r="J20" s="11">
         <f t="shared" si="10"/>
-        <v>-17.019545165380627</v>
+        <v>-14.394181464584459</v>
       </c>
       <c r="K20" s="11">
         <f t="shared" si="10"/>
-        <v>-33.517807278913793</v>
+        <v>-28.719816559195426</v>
       </c>
       <c r="L20" s="11">
         <f t="shared" si="10"/>
-        <v>-35.517500000000005</v>
+        <v>-30.175000000000004</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="10"/>
-        <v>-23.961216948152508</v>
+        <v>-19.756453630026488</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="10"/>
-        <v>-7.4629548346193753</v>
+        <v>-5.4308185354155425</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -2753,51 +2750,51 @@
       </c>
       <c r="C21" s="12">
         <f>C$9+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
-        <v>24.482500000000002</v>
+        <v>19.824999999999999</v>
       </c>
       <c r="D21" s="12">
         <f t="shared" ref="D21:N21" si="11">D$9+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
-        <v>18.44371694815252</v>
+        <v>14.5814536300265</v>
       </c>
       <c r="E21" s="12">
         <f t="shared" si="11"/>
-        <v>12.980454834619362</v>
+        <v>10.605818535415532</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="11"/>
-        <v>5.517500000000001</v>
+        <v>5.1750000000000007</v>
       </c>
       <c r="G21" s="12">
         <f t="shared" si="11"/>
-        <v>-7.4629548346193522</v>
+        <v>-5.4308185354155247</v>
       </c>
       <c r="H21" s="12">
         <f t="shared" si="11"/>
-        <v>-23.961216948152522</v>
+        <v>-19.756453630026499</v>
       </c>
       <c r="I21" s="12">
         <f t="shared" si="11"/>
-        <v>-35.517499999999998</v>
+        <v>-30.174999999999997</v>
       </c>
       <c r="J21" s="12">
         <f t="shared" si="11"/>
-        <v>-33.517807278913807</v>
+        <v>-28.71981655919544</v>
       </c>
       <c r="K21" s="12">
         <f t="shared" si="11"/>
-        <v>-17.019545165380663</v>
+        <v>-14.394181464584486</v>
       </c>
       <c r="L21" s="12">
         <f t="shared" si="11"/>
-        <v>5.5174999999999876</v>
+        <v>5.1749999999999883</v>
       </c>
       <c r="M21" s="12">
         <f t="shared" si="11"/>
-        <v>22.53704516538064</v>
+        <v>19.569181464584471</v>
       </c>
       <c r="N21" s="12">
         <f t="shared" si="11"/>
-        <v>28.000307278913795</v>
+        <v>23.544816559195429</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -2806,10 +2803,10 @@
       </c>
       <c r="C23">
         <f>E2/2</f>
-        <v>5.5175000000000001</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>19</v>
+        <v>5.1749999999999998</v>
+      </c>
+      <c r="D23" s="15">
+        <v>4.5</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final (or near so) designs for the Hallbach cylinder
</commit_message>
<xml_diff>
--- a/HalbachPositions (version 1).xlsx
+++ b/HalbachPositions (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steph\Documents\GitHub\Hallbach_cylinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DD17A4-DAA5-4761-9884-15AED1085CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54400E2-D61C-472D-B181-5619DC8994B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5A3979A9-2DE4-234A-B973-A6AC692A53E8}"/>
   </bookViews>
@@ -89,10 +89,10 @@
     <t>Ring height</t>
   </si>
   <si>
-    <t>Tolerance</t>
+    <t xml:space="preserve"> 0.004 inches</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.004 inches</t>
+    <t>Tolerance (manufacture's)</t>
   </si>
 </sst>
 </file>
@@ -393,40 +393,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.1749999999999998</c:v>
+                  <c:v>4.9749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.569181464584467</c:v>
+                  <c:v>19.295976383827579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.544816559195436</c:v>
+                  <c:v>23.47161147843855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.825000000000003</c:v>
+                  <c:v>20.025000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.581453630026498</c:v>
+                  <c:v>14.854658710783387</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.60581853541553</c:v>
+                  <c:v>10.679023616172417</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.1750000000000007</c:v>
+                  <c:v>4.9750000000000014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.430818535415523</c:v>
+                  <c:v>-5.7040236161724103</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-19.756453630026481</c:v>
+                  <c:v>-19.82965871078337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-30.174999999999994</c:v>
+                  <c:v>-29.974999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-28.719816559195433</c:v>
+                  <c:v>-28.446611478438545</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-14.394181464584481</c:v>
+                  <c:v>-14.320976383827594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,40 +438,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>30.174999999999997</c:v>
+                  <c:v>29.974999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.756453630026499</c:v>
+                  <c:v>19.829658710783388</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4308185354155354</c:v>
+                  <c:v>5.7040236161724227</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.174999999999998</c:v>
+                  <c:v>-4.9749999999999979</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-10.605818535415528</c:v>
+                  <c:v>-10.679023616172415</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-14.5814536300265</c:v>
+                  <c:v>-14.854658710783387</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-19.824999999999999</c:v>
+                  <c:v>-20.024999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-23.544816559195436</c:v>
+                  <c:v>-23.471611478438547</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-19.569181464584478</c:v>
+                  <c:v>-19.29597638382759</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.1750000000000096</c:v>
+                  <c:v>-4.9750000000000094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.394181464584481</c:v>
+                  <c:v>14.320976383827594</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.719816559195426</c:v>
+                  <c:v>28.446611478438541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,40 +522,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-5.1749999999999989</c:v>
+                  <c:v>-4.9749999999999988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.394181464584467</c:v>
+                  <c:v>14.320976383827579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.719816559195433</c:v>
+                  <c:v>28.446611478438548</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.175000000000001</c:v>
+                  <c:v>29.975000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.756453630026503</c:v>
+                  <c:v>19.829658710783391</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4308185354155292</c:v>
+                  <c:v>5.7040236161724165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.174999999999998</c:v>
+                  <c:v>-4.9749999999999979</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-10.605818535415526</c:v>
+                  <c:v>-10.679023616172415</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-14.581453630026491</c:v>
+                  <c:v>-14.854658710783379</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.824999999999996</c:v>
+                  <c:v>-20.024999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-23.544816559195443</c:v>
+                  <c:v>-23.471611478438554</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.569181464584478</c:v>
+                  <c:v>-19.295976383827593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,40 +567,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>30.175000000000001</c:v>
+                  <c:v>29.975000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.719816559195436</c:v>
+                  <c:v>28.446611478438552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.394181464584475</c:v>
+                  <c:v>14.320976383827587</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.1749999999999972</c:v>
+                  <c:v>-4.974999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-19.569181464584464</c:v>
+                  <c:v>-19.295976383827579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-23.544816559195439</c:v>
+                  <c:v>-23.47161147843855</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-19.825000000000003</c:v>
+                  <c:v>-20.025000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-14.581453630026498</c:v>
+                  <c:v>-14.854658710783387</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-10.605818535415535</c:v>
+                  <c:v>-10.679023616172422</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.1749999999999972</c:v>
+                  <c:v>-4.9749999999999979</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.4308185354155372</c:v>
+                  <c:v>5.7040236161724236</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.756453630026488</c:v>
+                  <c:v>19.829658710783374</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -651,40 +651,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-5.1749999999999998</c:v>
+                  <c:v>-4.9749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4308185354155292</c:v>
+                  <c:v>5.7040236161724165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.756453630026495</c:v>
+                  <c:v>19.829658710783381</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.174999999999997</c:v>
+                  <c:v>29.974999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.71981655919544</c:v>
+                  <c:v>28.446611478438552</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.394181464584467</c:v>
+                  <c:v>14.320976383827579</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.1749999999999954</c:v>
+                  <c:v>-4.9749999999999961</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-19.569181464584464</c:v>
+                  <c:v>-19.295976383827576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-23.544816559195436</c:v>
+                  <c:v>-23.471611478438547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.825000000000006</c:v>
+                  <c:v>-20.025000000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-14.581453630026498</c:v>
+                  <c:v>-14.854658710783387</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-10.605818535415541</c:v>
+                  <c:v>-10.679023616172428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -696,40 +696,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>19.825000000000003</c:v>
+                  <c:v>20.025000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.544816559195439</c:v>
+                  <c:v>23.47161147843855</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.569181464584471</c:v>
+                  <c:v>19.295976383827586</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1750000000000016</c:v>
+                  <c:v>4.9750000000000014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-14.394181464584461</c:v>
+                  <c:v>-14.320976383827574</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-28.719816559195436</c:v>
+                  <c:v>-28.446611478438552</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-30.175000000000001</c:v>
+                  <c:v>-29.975000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-19.756453630026503</c:v>
+                  <c:v>-19.829658710783391</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.4308185354155434</c:v>
+                  <c:v>-5.7040236161724307</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.1750000000000007</c:v>
+                  <c:v>4.9750000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.605818535415526</c:v>
+                  <c:v>10.679023616172413</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.581453630026491</c:v>
+                  <c:v>14.854658710783378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,40 +780,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.1749999999999989</c:v>
+                  <c:v>4.9749999999999988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.60581853541553</c:v>
+                  <c:v>10.679023616172417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.581453630026498</c:v>
+                  <c:v>14.854658710783385</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.824999999999999</c:v>
+                  <c:v>20.024999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.544816559195436</c:v>
+                  <c:v>23.471611478438547</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.569181464584467</c:v>
+                  <c:v>19.295976383827579</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.1750000000000034</c:v>
+                  <c:v>4.9750000000000032</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-14.394181464584459</c:v>
+                  <c:v>-14.320976383827571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-28.719816559195426</c:v>
+                  <c:v>-28.446611478438538</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-30.175000000000004</c:v>
+                  <c:v>-29.975000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-19.756453630026488</c:v>
+                  <c:v>-19.829658710783377</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-5.4308185354155425</c:v>
+                  <c:v>-5.7040236161724298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,40 +825,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>19.824999999999999</c:v>
+                  <c:v>20.024999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.5814536300265</c:v>
+                  <c:v>14.854658710783387</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.605818535415532</c:v>
+                  <c:v>10.679023616172421</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1750000000000007</c:v>
+                  <c:v>4.9750000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.4308185354155247</c:v>
+                  <c:v>-5.704023616172412</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-19.756453630026499</c:v>
+                  <c:v>-19.829658710783388</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-30.174999999999997</c:v>
+                  <c:v>-29.974999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-28.71981655919544</c:v>
+                  <c:v>-28.446611478438552</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-14.394181464584486</c:v>
+                  <c:v>-14.320976383827599</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.1749999999999883</c:v>
+                  <c:v>4.974999999999989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.569181464584471</c:v>
+                  <c:v>19.295976383827583</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.544816559195429</c:v>
+                  <c:v>23.471611478438543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,7 +2052,7 @@
   <dimension ref="B2:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2071,7 +2071,7 @@
         <v>16</v>
       </c>
       <c r="E2">
-        <v>10.35</v>
+        <v>9.9499999999999993</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -2385,51 +2385,51 @@
       </c>
       <c r="C14" s="5">
         <f>C$8+($E$2/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
-        <v>5.1749999999999998</v>
+        <v>4.9749999999999996</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" ref="D14:N14" si="4">D$8+($E$2/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
-        <v>19.569181464584467</v>
+        <v>19.295976383827579</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="4"/>
-        <v>23.544816559195436</v>
+        <v>23.47161147843855</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="4"/>
-        <v>19.825000000000003</v>
+        <v>20.025000000000002</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="4"/>
-        <v>14.581453630026498</v>
+        <v>14.854658710783387</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>10.60581853541553</v>
+        <v>10.679023616172417</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="4"/>
-        <v>5.1750000000000007</v>
+        <v>4.9750000000000014</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="4"/>
-        <v>-5.430818535415523</v>
+        <v>-5.7040236161724103</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="4"/>
-        <v>-19.756453630026481</v>
+        <v>-19.82965871078337</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="4"/>
-        <v>-30.174999999999994</v>
+        <v>-29.974999999999994</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="4"/>
-        <v>-28.719816559195433</v>
+        <v>-28.446611478438545</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="4"/>
-        <v>-14.394181464584481</v>
+        <v>-14.320976383827594</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -2438,51 +2438,51 @@
       </c>
       <c r="C15" s="6">
         <f>C$9+($E$2/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
-        <v>30.174999999999997</v>
+        <v>29.974999999999998</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" ref="D15:N15" si="5">D$9+($E$2/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
-        <v>19.756453630026499</v>
+        <v>19.829658710783388</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="5"/>
-        <v>5.4308185354155354</v>
+        <v>5.7040236161724227</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" si="5"/>
-        <v>-5.174999999999998</v>
+        <v>-4.9749999999999979</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" si="5"/>
-        <v>-10.605818535415528</v>
+        <v>-10.679023616172415</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="5"/>
-        <v>-14.5814536300265</v>
+        <v>-14.854658710783387</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="5"/>
-        <v>-19.824999999999999</v>
+        <v>-20.024999999999999</v>
       </c>
       <c r="J15" s="6">
         <f t="shared" si="5"/>
-        <v>-23.544816559195436</v>
+        <v>-23.471611478438547</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="5"/>
-        <v>-19.569181464584478</v>
+        <v>-19.29597638382759</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="5"/>
-        <v>-5.1750000000000096</v>
+        <v>-4.9750000000000094</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="5"/>
-        <v>14.394181464584481</v>
+        <v>14.320976383827594</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="5"/>
-        <v>28.719816559195426</v>
+        <v>28.446611478438541</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -2491,51 +2491,51 @@
       </c>
       <c r="C16" s="7">
         <f>C$8+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
-        <v>-5.1749999999999989</v>
+        <v>-4.9749999999999988</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" ref="D16:N16" si="6">D$8+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
-        <v>14.394181464584467</v>
+        <v>14.320976383827579</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="6"/>
-        <v>28.719816559195433</v>
+        <v>28.446611478438548</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="6"/>
-        <v>30.175000000000001</v>
+        <v>29.975000000000001</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="6"/>
-        <v>19.756453630026503</v>
+        <v>19.829658710783391</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="6"/>
-        <v>5.4308185354155292</v>
+        <v>5.7040236161724165</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" si="6"/>
-        <v>-5.174999999999998</v>
+        <v>-4.9749999999999979</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" si="6"/>
-        <v>-10.605818535415526</v>
+        <v>-10.679023616172415</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="6"/>
-        <v>-14.581453630026491</v>
+        <v>-14.854658710783379</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="6"/>
-        <v>-19.824999999999996</v>
+        <v>-20.024999999999995</v>
       </c>
       <c r="M16" s="7">
         <f t="shared" si="6"/>
-        <v>-23.544816559195443</v>
+        <v>-23.471611478438554</v>
       </c>
       <c r="N16" s="7">
         <f t="shared" si="6"/>
-        <v>-19.569181464584478</v>
+        <v>-19.295976383827593</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -2544,51 +2544,51 @@
       </c>
       <c r="C17" s="8">
         <f>C$9+($E$2/(2^0.5))*COS((PI()/4)-(2*C$7))</f>
-        <v>30.175000000000001</v>
+        <v>29.975000000000001</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" ref="D17:N17" si="7">D$9+($E$2/(2^0.5))*COS((PI()/4)-(2*D$7))</f>
-        <v>28.719816559195436</v>
+        <v>28.446611478438552</v>
       </c>
       <c r="E17" s="8">
         <f t="shared" si="7"/>
-        <v>14.394181464584475</v>
+        <v>14.320976383827587</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="7"/>
-        <v>-5.1749999999999972</v>
+        <v>-4.974999999999997</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="7"/>
-        <v>-19.569181464584464</v>
+        <v>-19.295976383827579</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="7"/>
-        <v>-23.544816559195439</v>
+        <v>-23.47161147843855</v>
       </c>
       <c r="I17" s="8">
         <f t="shared" si="7"/>
-        <v>-19.825000000000003</v>
+        <v>-20.025000000000002</v>
       </c>
       <c r="J17" s="8">
         <f t="shared" si="7"/>
-        <v>-14.581453630026498</v>
+        <v>-14.854658710783387</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="7"/>
-        <v>-10.605818535415535</v>
+        <v>-10.679023616172422</v>
       </c>
       <c r="L17" s="8">
         <f t="shared" si="7"/>
-        <v>-5.1749999999999972</v>
+        <v>-4.9749999999999979</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" si="7"/>
-        <v>5.4308185354155372</v>
+        <v>5.7040236161724236</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" si="7"/>
-        <v>19.756453630026488</v>
+        <v>19.829658710783374</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -2597,51 +2597,51 @@
       </c>
       <c r="C18" s="9">
         <f>C$8+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
-        <v>-5.1749999999999998</v>
+        <v>-4.9749999999999996</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" ref="D18:N18" si="8">D$8+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
-        <v>5.4308185354155292</v>
+        <v>5.7040236161724165</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="8"/>
-        <v>19.756453630026495</v>
+        <v>19.829658710783381</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="8"/>
-        <v>30.174999999999997</v>
+        <v>29.974999999999998</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="8"/>
-        <v>28.71981655919544</v>
+        <v>28.446611478438552</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" si="8"/>
-        <v>14.394181464584467</v>
+        <v>14.320976383827579</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="8"/>
-        <v>-5.1749999999999954</v>
+        <v>-4.9749999999999961</v>
       </c>
       <c r="J18" s="9">
         <f t="shared" si="8"/>
-        <v>-19.569181464584464</v>
+        <v>-19.295976383827576</v>
       </c>
       <c r="K18" s="9">
         <f t="shared" si="8"/>
-        <v>-23.544816559195436</v>
+        <v>-23.471611478438547</v>
       </c>
       <c r="L18" s="9">
         <f t="shared" si="8"/>
-        <v>-19.825000000000006</v>
+        <v>-20.025000000000006</v>
       </c>
       <c r="M18" s="9">
         <f t="shared" si="8"/>
-        <v>-14.581453630026498</v>
+        <v>-14.854658710783387</v>
       </c>
       <c r="N18" s="9">
         <f t="shared" si="8"/>
-        <v>-10.605818535415541</v>
+        <v>-10.679023616172428</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -2650,51 +2650,51 @@
       </c>
       <c r="C19" s="10">
         <f>C$9+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*C$7))</f>
-        <v>19.825000000000003</v>
+        <v>20.025000000000002</v>
       </c>
       <c r="D19" s="10">
         <f t="shared" ref="D19:N19" si="9">D$9+($E$2/(2^0.5))*(-1)*SIN((PI()/4)-(2*D$7))</f>
-        <v>23.544816559195439</v>
+        <v>23.47161147843855</v>
       </c>
       <c r="E19" s="10">
         <f t="shared" si="9"/>
-        <v>19.569181464584471</v>
+        <v>19.295976383827586</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="9"/>
-        <v>5.1750000000000016</v>
+        <v>4.9750000000000014</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" si="9"/>
-        <v>-14.394181464584461</v>
+        <v>-14.320976383827574</v>
       </c>
       <c r="H19" s="10">
         <f t="shared" si="9"/>
-        <v>-28.719816559195436</v>
+        <v>-28.446611478438552</v>
       </c>
       <c r="I19" s="10">
         <f t="shared" si="9"/>
-        <v>-30.175000000000001</v>
+        <v>-29.975000000000001</v>
       </c>
       <c r="J19" s="10">
         <f t="shared" si="9"/>
-        <v>-19.756453630026503</v>
+        <v>-19.829658710783391</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="9"/>
-        <v>-5.4308185354155434</v>
+        <v>-5.7040236161724307</v>
       </c>
       <c r="L19" s="10">
         <f t="shared" si="9"/>
-        <v>5.1750000000000007</v>
+        <v>4.9750000000000005</v>
       </c>
       <c r="M19" s="10">
         <f t="shared" si="9"/>
-        <v>10.605818535415526</v>
+        <v>10.679023616172413</v>
       </c>
       <c r="N19" s="10">
         <f t="shared" si="9"/>
-        <v>14.581453630026491</v>
+        <v>14.854658710783378</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -2703,51 +2703,51 @@
       </c>
       <c r="C20" s="11">
         <f>C$8+($E$2/(2^0.5))*SIN((PI()/4)-(2*C$7))</f>
-        <v>5.1749999999999989</v>
+        <v>4.9749999999999988</v>
       </c>
       <c r="D20" s="11">
         <f t="shared" ref="D20:N20" si="10">D$8+($E$2/(2^0.5))*SIN((PI()/4)-(2*D$7))</f>
-        <v>10.60581853541553</v>
+        <v>10.679023616172417</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="10"/>
-        <v>14.581453630026498</v>
+        <v>14.854658710783385</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="10"/>
-        <v>19.824999999999999</v>
+        <v>20.024999999999999</v>
       </c>
       <c r="G20" s="11">
         <f t="shared" si="10"/>
-        <v>23.544816559195436</v>
+        <v>23.471611478438547</v>
       </c>
       <c r="H20" s="11">
         <f t="shared" si="10"/>
-        <v>19.569181464584467</v>
+        <v>19.295976383827579</v>
       </c>
       <c r="I20" s="11">
         <f t="shared" si="10"/>
-        <v>5.1750000000000034</v>
+        <v>4.9750000000000032</v>
       </c>
       <c r="J20" s="11">
         <f t="shared" si="10"/>
-        <v>-14.394181464584459</v>
+        <v>-14.320976383827571</v>
       </c>
       <c r="K20" s="11">
         <f t="shared" si="10"/>
-        <v>-28.719816559195426</v>
+        <v>-28.446611478438538</v>
       </c>
       <c r="L20" s="11">
         <f t="shared" si="10"/>
-        <v>-30.175000000000004</v>
+        <v>-29.975000000000005</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="10"/>
-        <v>-19.756453630026488</v>
+        <v>-19.829658710783377</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="10"/>
-        <v>-5.4308185354155425</v>
+        <v>-5.7040236161724298</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -2756,51 +2756,51 @@
       </c>
       <c r="C21" s="12">
         <f>C$9+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*C$7))</f>
-        <v>19.824999999999999</v>
+        <v>20.024999999999999</v>
       </c>
       <c r="D21" s="12">
         <f t="shared" ref="D21:N21" si="11">D$9+($E$2/(2^0.5))*(-1)*COS((PI()/4)-(2*D$7))</f>
-        <v>14.5814536300265</v>
+        <v>14.854658710783387</v>
       </c>
       <c r="E21" s="12">
         <f t="shared" si="11"/>
-        <v>10.605818535415532</v>
+        <v>10.679023616172421</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="11"/>
-        <v>5.1750000000000007</v>
+        <v>4.9750000000000005</v>
       </c>
       <c r="G21" s="12">
         <f t="shared" si="11"/>
-        <v>-5.4308185354155247</v>
+        <v>-5.704023616172412</v>
       </c>
       <c r="H21" s="12">
         <f t="shared" si="11"/>
-        <v>-19.756453630026499</v>
+        <v>-19.829658710783388</v>
       </c>
       <c r="I21" s="12">
         <f t="shared" si="11"/>
-        <v>-30.174999999999997</v>
+        <v>-29.974999999999998</v>
       </c>
       <c r="J21" s="12">
         <f t="shared" si="11"/>
-        <v>-28.71981655919544</v>
+        <v>-28.446611478438552</v>
       </c>
       <c r="K21" s="12">
         <f t="shared" si="11"/>
-        <v>-14.394181464584486</v>
+        <v>-14.320976383827599</v>
       </c>
       <c r="L21" s="12">
         <f t="shared" si="11"/>
-        <v>5.1749999999999883</v>
+        <v>4.974999999999989</v>
       </c>
       <c r="M21" s="12">
         <f t="shared" si="11"/>
-        <v>19.569181464584471</v>
+        <v>19.295976383827583</v>
       </c>
       <c r="N21" s="12">
         <f t="shared" si="11"/>
-        <v>23.544816559195429</v>
+        <v>23.471611478438543</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="C23">
         <f>E2/2</f>
-        <v>5.1749999999999998</v>
+        <v>4.9749999999999996</v>
       </c>
       <c r="D23" s="15">
         <v>4.5</v>
@@ -2825,10 +2825,10 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
         <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>